<commit_message>
getPrices Update -> bloqued page or no price found = different value
</commit_message>
<xml_diff>
--- a/excelPriceCards/cartes_url.xlsx
+++ b/excelPriceCards/cartes_url.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Nom</t>
   </si>
@@ -52,24 +52,6 @@
     <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-VMAX-V1</t>
   </si>
   <si>
-    <t>Nymphali</t>
-  </si>
-  <si>
-    <t>41/69</t>
-  </si>
-  <si>
-    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041</t>
-  </si>
-  <si>
-    <t>Nocatli</t>
-  </si>
-  <si>
-    <t>48/69</t>
-  </si>
-  <si>
-    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1</t>
-  </si>
-  <si>
     <t>Giratina Holo</t>
   </si>
   <si>
@@ -83,6 +65,72 @@
   </si>
   <si>
     <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Platinum/Giratina-Lv63-PL10</t>
+  </si>
+  <si>
+    <t>Giratina VSTAR</t>
+  </si>
+  <si>
+    <t>261/172</t>
+  </si>
+  <si>
+    <t>S12A</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261</t>
+  </si>
+  <si>
+    <t>Energie Tênebre</t>
+  </si>
+  <si>
+    <t>257/172</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkness-Energy-s12a257</t>
+  </si>
+  <si>
+    <t>Energie Acier</t>
+  </si>
+  <si>
+    <t>258/172</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Metal-Energy-s12a258</t>
+  </si>
+  <si>
+    <t>Energie Feu</t>
+  </si>
+  <si>
+    <t>252/172</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Fire-Energy-s12a252</t>
+  </si>
+  <si>
+    <t>Regigigas VSTAR</t>
+  </si>
+  <si>
+    <t>233/172</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233</t>
+  </si>
+  <si>
+    <t>Entei V</t>
+  </si>
+  <si>
+    <t>213/172</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213</t>
+  </si>
+  <si>
+    <t>Charisme de Giovanni</t>
+  </si>
+  <si>
+    <t>204/165</t>
+  </si>
+  <si>
+    <t>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204</t>
   </si>
 </sst>
 </file>
@@ -90,19 +138,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,14 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -137,13 +172,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -448,7 +483,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -458,8 +493,7 @@
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="62.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="46.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -476,7 +510,6 @@
         <v>3</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
@@ -494,7 +527,6 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
@@ -512,7 +544,6 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
@@ -522,51 +553,133 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2">
+        <v>151</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>